<commit_message>
P05 Task1 MXF mv Mice.java Scoop
</commit_message>
<xml_diff>
--- a/P05/Scrum_MICE.xlsx
+++ b/P05/Scrum_MICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aliya\Desktop\UTA\Courses\2022\2nd Fall 2022\CSE\CSE-1325-001 (Java)\HW\P05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aliya\Desktop\vmh_share3RD\2022\Practice\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="182">
   <si>
     <t>Product Name:</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>In Work</t>
+  </si>
+  <si>
+    <t>mv Mice.java Scoop</t>
   </si>
 </sst>
 </file>
@@ -1071,11 +1074,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146537128"/>
-        <c:axId val="146535560"/>
+        <c:axId val="146292784"/>
+        <c:axId val="146293176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146537128"/>
+        <c:axId val="146292784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1135,12 +1138,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146535560"/>
+        <c:crossAx val="146293176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146535560"/>
+        <c:axId val="146293176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1208,7 +1211,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146537128"/>
+        <c:crossAx val="146292784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1338,28 +1341,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,11 +1390,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="146536736"/>
-        <c:axId val="146542616"/>
+        <c:axId val="174947664"/>
+        <c:axId val="174952368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146536736"/>
+        <c:axId val="174947664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146542616"/>
+        <c:crossAx val="174952368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1457,7 +1460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146542616"/>
+        <c:axId val="174952368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146536736"/>
+        <c:crossAx val="174947664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1702,11 +1705,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="146542224"/>
-        <c:axId val="146543008"/>
+        <c:axId val="174948448"/>
+        <c:axId val="174948840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146542224"/>
+        <c:axId val="174948448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146543008"/>
+        <c:crossAx val="174948840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +1774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146543008"/>
+        <c:axId val="174948840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,7 +1840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146542224"/>
+        <c:crossAx val="174948448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2015,11 +2018,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="146535952"/>
-        <c:axId val="146539088"/>
+        <c:axId val="174949232"/>
+        <c:axId val="174953544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146535952"/>
+        <c:axId val="174949232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +2079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146539088"/>
+        <c:crossAx val="174953544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2084,7 +2087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146539088"/>
+        <c:axId val="174953544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,7 +2153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146535952"/>
+        <c:crossAx val="174949232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2328,11 +2331,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="146536344"/>
-        <c:axId val="146539872"/>
+        <c:axId val="174949624"/>
+        <c:axId val="174946488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146536344"/>
+        <c:axId val="174949624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,7 +2392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146539872"/>
+        <c:crossAx val="174946488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2397,7 +2400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146539872"/>
+        <c:axId val="174946488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2463,7 +2466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146536344"/>
+        <c:crossAx val="174949624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2641,11 +2644,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="172025848"/>
-        <c:axId val="172028592"/>
+        <c:axId val="174950800"/>
+        <c:axId val="174946880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172025848"/>
+        <c:axId val="174950800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,7 +2705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172028592"/>
+        <c:crossAx val="174946880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2710,7 +2713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172028592"/>
+        <c:axId val="174946880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2776,7 +2779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172025848"/>
+        <c:crossAx val="174950800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2954,11 +2957,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="172028984"/>
-        <c:axId val="172027024"/>
+        <c:axId val="174951584"/>
+        <c:axId val="174952760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="172028984"/>
+        <c:axId val="174951584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3015,7 +3018,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172027024"/>
+        <c:crossAx val="174952760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3023,7 +3026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172027024"/>
+        <c:axId val="174952760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3089,7 +3092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172028984"/>
+        <c:crossAx val="174951584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3142,7 +3145,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3183,7 +3186,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3224,7 +3227,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,7 +3268,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3306,7 +3309,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3347,7 +3350,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3388,7 +3391,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5679,7 +5682,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -5781,7 +5784,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -5796,7 +5799,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5814,7 +5817,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5832,7 +5835,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5850,7 +5853,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5868,7 +5871,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5886,7 +5889,7 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5904,7 +5907,7 @@
       </c>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5982,9 +5985,18 @@
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">

</xml_diff>

<commit_message>
P05 Task5 Revised MixIn
</commit_message>
<xml_diff>
--- a/P05/Scrum_MICE.xlsx
+++ b/P05/Scrum_MICE.xlsx
@@ -25,8 +25,56 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="D17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "Task1 MX InWork"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P05 Task4 MixIn resolved"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P05 Task5 Revised MixIn"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="185">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -565,7 +613,16 @@
     <t xml:space="preserve">In Work</t>
   </si>
   <si>
+    <t xml:space="preserve">git commit -m "P05 Task1 MXF MixInFlavor &amp; IceCreamFlavor"</t>
+  </si>
+  <si>
     <t xml:space="preserve">mv Mice.java Scoop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MixIn resolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revised MixIn</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -584,7 +641,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ dd"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -698,6 +755,11 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -987,1537 +1049,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="62975676"/>
-        <c:axId val="60806490"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="62975676"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="60806490"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="60806490"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="62975676"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="6207492"/>
-        <c:axId val="17314906"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="6207492"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="17314906"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="17314906"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="6207492"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 04 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="23868528"/>
-        <c:axId val="40313240"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="23868528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="40313240"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="40313240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="23868528"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 05 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="57840883"/>
-        <c:axId val="42421951"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="57840883"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="42421951"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="42421951"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="57840883"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 06 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="68407623"/>
-        <c:axId val="58247379"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="68407623"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="58247379"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="58247379"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="68407623"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2675,11 +1207,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="69427237"/>
-        <c:axId val="79543373"/>
+        <c:axId val="3921322"/>
+        <c:axId val="20101124"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69427237"/>
+        <c:axId val="3921322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2746,12 +1278,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79543373"/>
+        <c:crossAx val="20101124"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79543373"/>
+        <c:axId val="20101124"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2826,7 +1358,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69427237"/>
+        <c:crossAx val="3921322"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2853,7 +1385,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2945,28 +1477,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2981,11 +1513,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="70088390"/>
-        <c:axId val="40166332"/>
+        <c:axId val="10330309"/>
+        <c:axId val="25002496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70088390"/>
+        <c:axId val="10330309"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3050,7 +1582,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40166332"/>
+        <c:crossAx val="25002496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3058,7 +1590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40166332"/>
+        <c:axId val="25002496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,7 +1664,1537 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70088390"/>
+        <c:crossAx val="10330309"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart80.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="26090149"/>
+        <c:axId val="4449694"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="26090149"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4449694"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="4449694"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="26090149"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart81.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="36415757"/>
+        <c:axId val="12844541"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="36415757"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12844541"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="12844541"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="36415757"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart82.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 04 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="44912799"/>
+        <c:axId val="39701550"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="44912799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39701550"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39701550"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44912799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart83.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 05 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="47661159"/>
+        <c:axId val="39374839"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="47661159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39374839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39374839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47661159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart84.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 06 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="49924952"/>
+        <c:axId val="76405830"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49924952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76405830"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="76405830"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="49924952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3412,8 +3474,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5338,7 +5400,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5427,7 +5489,7 @@
       </c>
       <c r="B7" s="21" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -5440,7 +5502,7 @@
       </c>
       <c r="B8" s="21" t="n">
         <f aca="false">B7-C8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5456,7 +5518,7 @@
       </c>
       <c r="B9" s="21" t="n">
         <f aca="false">B8-C9</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5472,7 +5534,7 @@
       </c>
       <c r="B10" s="21" t="n">
         <f aca="false">B9-C10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5488,7 +5550,7 @@
       </c>
       <c r="B11" s="21" t="n">
         <f aca="false">B10-C11</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5504,7 +5566,7 @@
       </c>
       <c r="B12" s="21" t="n">
         <f aca="false">B11-C12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5520,7 +5582,7 @@
       </c>
       <c r="B13" s="21" t="n">
         <f aca="false">B12-C13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C13" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5536,7 +5598,7 @@
       </c>
       <c r="B14" s="21" t="n">
         <f aca="false">B13-C14</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5574,7 +5636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
@@ -5601,7 +5663,9 @@
       <c r="C18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="33"/>
+      <c r="D18" s="29" t="s">
+        <v>179</v>
+      </c>
       <c r="E18" s="32" t="s">
         <v>178</v>
       </c>
@@ -5616,29 +5680,43 @@
       <c r="C19" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>179</v>
+      <c r="D19" s="29" t="s">
+        <v>180</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="33"/>
+      <c r="B21" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="E21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5647,7 +5725,7 @@
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="30"/>
-      <c r="D22" s="33"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5656,7 +5734,7 @@
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="30"/>
-      <c r="D23" s="33"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,7 +5743,7 @@
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="33"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,7 +5752,7 @@
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="30"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5683,7 +5761,7 @@
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="30"/>
-      <c r="D26" s="33"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5692,7 +5770,7 @@
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="30"/>
-      <c r="D27" s="33"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5701,7 +5779,7 @@
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="30"/>
-      <c r="D28" s="33"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5710,7 +5788,7 @@
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="30"/>
-      <c r="D29" s="33"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5719,7 +5797,7 @@
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="30"/>
-      <c r="D30" s="33"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5728,7 +5806,7 @@
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="30"/>
-      <c r="D31" s="33"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5737,7 +5815,7 @@
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="30"/>
-      <c r="D32" s="33"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5746,7 +5824,7 @@
       </c>
       <c r="B33" s="29"/>
       <c r="C33" s="30"/>
-      <c r="D33" s="33"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5755,7 +5833,7 @@
       </c>
       <c r="B34" s="29"/>
       <c r="C34" s="30"/>
-      <c r="D34" s="33"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5764,7 +5842,7 @@
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="30"/>
-      <c r="D35" s="33"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5773,7 +5851,7 @@
       </c>
       <c r="B36" s="29"/>
       <c r="C36" s="30"/>
-      <c r="D36" s="33"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5782,7 +5860,7 @@
       </c>
       <c r="B37" s="29"/>
       <c r="C37" s="30"/>
-      <c r="D37" s="33"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,7 +5869,7 @@
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="30"/>
-      <c r="D38" s="33"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5800,7 +5878,7 @@
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="30"/>
-      <c r="D39" s="33"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5809,7 +5887,7 @@
       </c>
       <c r="B40" s="29"/>
       <c r="C40" s="30"/>
-      <c r="D40" s="33"/>
+      <c r="D40" s="29"/>
       <c r="E40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5818,7 +5896,7 @@
       </c>
       <c r="B41" s="29"/>
       <c r="C41" s="30"/>
-      <c r="D41" s="33"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5827,7 +5905,7 @@
       </c>
       <c r="B42" s="29"/>
       <c r="C42" s="30"/>
-      <c r="D42" s="33"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +5914,7 @@
       </c>
       <c r="B43" s="29"/>
       <c r="C43" s="30"/>
-      <c r="D43" s="33"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5845,7 +5923,7 @@
       </c>
       <c r="B44" s="29"/>
       <c r="C44" s="30"/>
-      <c r="D44" s="33"/>
+      <c r="D44" s="29"/>
       <c r="E44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5854,7 +5932,7 @@
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="30"/>
-      <c r="D45" s="33"/>
+      <c r="D45" s="29"/>
       <c r="E45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5863,7 +5941,7 @@
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="30"/>
-      <c r="D46" s="33"/>
+      <c r="D46" s="29"/>
       <c r="E46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5872,7 +5950,7 @@
       </c>
       <c r="B47" s="29"/>
       <c r="C47" s="30"/>
-      <c r="D47" s="33"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,7 +5959,7 @@
       </c>
       <c r="B48" s="29"/>
       <c r="C48" s="30"/>
-      <c r="D48" s="33"/>
+      <c r="D48" s="29"/>
       <c r="E48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5890,7 +5968,7 @@
       </c>
       <c r="B49" s="29"/>
       <c r="C49" s="30"/>
-      <c r="D49" s="33"/>
+      <c r="D49" s="29"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5899,7 +5977,7 @@
       </c>
       <c r="B50" s="29"/>
       <c r="C50" s="30"/>
-      <c r="D50" s="33"/>
+      <c r="D50" s="29"/>
       <c r="E50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5908,7 +5986,7 @@
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="33"/>
+      <c r="D51" s="29"/>
       <c r="E51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5917,7 +5995,7 @@
       </c>
       <c r="B52" s="29"/>
       <c r="C52" s="30"/>
-      <c r="D52" s="33"/>
+      <c r="D52" s="29"/>
       <c r="E52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5926,7 +6004,7 @@
       </c>
       <c r="B53" s="29"/>
       <c r="C53" s="30"/>
-      <c r="D53" s="33"/>
+      <c r="D53" s="29"/>
       <c r="E53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5935,7 +6013,7 @@
       </c>
       <c r="B54" s="29"/>
       <c r="C54" s="30"/>
-      <c r="D54" s="33"/>
+      <c r="D54" s="29"/>
       <c r="E54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5944,7 +6022,7 @@
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="30"/>
-      <c r="D55" s="33"/>
+      <c r="D55" s="29"/>
       <c r="E55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5953,7 +6031,7 @@
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="30"/>
-      <c r="D56" s="33"/>
+      <c r="D56" s="29"/>
       <c r="E56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,7 +6040,7 @@
       </c>
       <c r="B57" s="29"/>
       <c r="C57" s="30"/>
-      <c r="D57" s="33"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="32"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5971,7 +6049,7 @@
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="30"/>
-      <c r="D58" s="33"/>
+      <c r="D58" s="29"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5980,7 +6058,7 @@
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="30"/>
-      <c r="D59" s="33"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5989,7 +6067,7 @@
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="30"/>
-      <c r="D60" s="33"/>
+      <c r="D60" s="29"/>
       <c r="E60" s="32"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,7 +6076,7 @@
       </c>
       <c r="B61" s="29"/>
       <c r="C61" s="30"/>
-      <c r="D61" s="33"/>
+      <c r="D61" s="29"/>
       <c r="E61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6007,7 +6085,7 @@
       </c>
       <c r="B62" s="29"/>
       <c r="C62" s="30"/>
-      <c r="D62" s="33"/>
+      <c r="D62" s="29"/>
       <c r="E62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6016,7 +6094,7 @@
       </c>
       <c r="B63" s="29"/>
       <c r="C63" s="30"/>
-      <c r="D63" s="33"/>
+      <c r="D63" s="29"/>
       <c r="E63" s="32"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6025,7 +6103,7 @@
       </c>
       <c r="B64" s="29"/>
       <c r="C64" s="30"/>
-      <c r="D64" s="33"/>
+      <c r="D64" s="29"/>
       <c r="E64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6034,7 +6112,7 @@
       </c>
       <c r="B65" s="29"/>
       <c r="C65" s="30"/>
-      <c r="D65" s="33"/>
+      <c r="D65" s="29"/>
       <c r="E65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,7 +6121,7 @@
       </c>
       <c r="B66" s="29"/>
       <c r="C66" s="30"/>
-      <c r="D66" s="33"/>
+      <c r="D66" s="29"/>
       <c r="E66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6052,7 +6130,7 @@
       </c>
       <c r="B67" s="29"/>
       <c r="C67" s="30"/>
-      <c r="D67" s="33"/>
+      <c r="D67" s="29"/>
       <c r="E67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6061,7 +6139,7 @@
       </c>
       <c r="B68" s="29"/>
       <c r="C68" s="30"/>
-      <c r="D68" s="33"/>
+      <c r="D68" s="29"/>
       <c r="E68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6070,7 +6148,7 @@
       </c>
       <c r="B69" s="29"/>
       <c r="C69" s="30"/>
-      <c r="D69" s="33"/>
+      <c r="D69" s="29"/>
       <c r="E69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6079,7 +6157,7 @@
       </c>
       <c r="B70" s="29"/>
       <c r="C70" s="30"/>
-      <c r="D70" s="33"/>
+      <c r="D70" s="29"/>
       <c r="E70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6088,7 +6166,7 @@
       </c>
       <c r="B71" s="29"/>
       <c r="C71" s="30"/>
-      <c r="D71" s="33"/>
+      <c r="D71" s="29"/>
       <c r="E71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6097,7 +6175,7 @@
       </c>
       <c r="B72" s="29"/>
       <c r="C72" s="30"/>
-      <c r="D72" s="33"/>
+      <c r="D72" s="29"/>
       <c r="E72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6106,7 +6184,7 @@
       </c>
       <c r="B73" s="29"/>
       <c r="C73" s="30"/>
-      <c r="D73" s="33"/>
+      <c r="D73" s="29"/>
       <c r="E73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6115,7 +6193,7 @@
       </c>
       <c r="B74" s="29"/>
       <c r="C74" s="30"/>
-      <c r="D74" s="33"/>
+      <c r="D74" s="29"/>
       <c r="E74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6124,7 +6202,7 @@
       </c>
       <c r="B75" s="29"/>
       <c r="C75" s="30"/>
-      <c r="D75" s="33"/>
+      <c r="D75" s="29"/>
       <c r="E75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6133,7 +6211,7 @@
       </c>
       <c r="B76" s="29"/>
       <c r="C76" s="30"/>
-      <c r="D76" s="33"/>
+      <c r="D76" s="29"/>
       <c r="E76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6142,7 +6220,7 @@
       </c>
       <c r="B77" s="29"/>
       <c r="C77" s="30"/>
-      <c r="D77" s="33"/>
+      <c r="D77" s="29"/>
       <c r="E77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6151,7 +6229,7 @@
       </c>
       <c r="B78" s="29"/>
       <c r="C78" s="30"/>
-      <c r="D78" s="33"/>
+      <c r="D78" s="29"/>
       <c r="E78" s="32"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6160,7 +6238,7 @@
       </c>
       <c r="B79" s="29"/>
       <c r="C79" s="30"/>
-      <c r="D79" s="33"/>
+      <c r="D79" s="29"/>
       <c r="E79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6169,7 +6247,7 @@
       </c>
       <c r="B80" s="29"/>
       <c r="C80" s="30"/>
-      <c r="D80" s="33"/>
+      <c r="D80" s="29"/>
       <c r="E80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6178,7 +6256,7 @@
       </c>
       <c r="B81" s="29"/>
       <c r="C81" s="30"/>
-      <c r="D81" s="33"/>
+      <c r="D81" s="29"/>
       <c r="E81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6187,7 +6265,7 @@
       </c>
       <c r="B82" s="29"/>
       <c r="C82" s="30"/>
-      <c r="D82" s="33"/>
+      <c r="D82" s="29"/>
       <c r="E82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6196,7 +6274,7 @@
       </c>
       <c r="B83" s="29"/>
       <c r="C83" s="30"/>
-      <c r="D83" s="33"/>
+      <c r="D83" s="29"/>
       <c r="E83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6205,7 +6283,7 @@
       </c>
       <c r="B84" s="29"/>
       <c r="C84" s="30"/>
-      <c r="D84" s="33"/>
+      <c r="D84" s="29"/>
       <c r="E84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6214,7 +6292,7 @@
       </c>
       <c r="B85" s="29"/>
       <c r="C85" s="30"/>
-      <c r="D85" s="33"/>
+      <c r="D85" s="29"/>
       <c r="E85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6223,7 +6301,7 @@
       </c>
       <c r="B86" s="29"/>
       <c r="C86" s="30"/>
-      <c r="D86" s="33"/>
+      <c r="D86" s="29"/>
       <c r="E86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6232,7 +6310,7 @@
       </c>
       <c r="B87" s="29"/>
       <c r="C87" s="30"/>
-      <c r="D87" s="33"/>
+      <c r="D87" s="29"/>
       <c r="E87" s="32"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6241,7 +6319,7 @@
       </c>
       <c r="B88" s="29"/>
       <c r="C88" s="30"/>
-      <c r="D88" s="33"/>
+      <c r="D88" s="29"/>
       <c r="E88" s="32"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6250,7 +6328,7 @@
       </c>
       <c r="B89" s="29"/>
       <c r="C89" s="30"/>
-      <c r="D89" s="33"/>
+      <c r="D89" s="29"/>
       <c r="E89" s="32"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6259,7 +6337,7 @@
       </c>
       <c r="B90" s="29"/>
       <c r="C90" s="30"/>
-      <c r="D90" s="33"/>
+      <c r="D90" s="29"/>
       <c r="E90" s="32"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6268,7 +6346,7 @@
       </c>
       <c r="B91" s="29"/>
       <c r="C91" s="30"/>
-      <c r="D91" s="33"/>
+      <c r="D91" s="29"/>
       <c r="E91" s="32"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,7 +6355,7 @@
       </c>
       <c r="B92" s="29"/>
       <c r="C92" s="30"/>
-      <c r="D92" s="33"/>
+      <c r="D92" s="29"/>
       <c r="E92" s="32"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6286,7 +6364,7 @@
       </c>
       <c r="B93" s="29"/>
       <c r="C93" s="30"/>
-      <c r="D93" s="33"/>
+      <c r="D93" s="29"/>
       <c r="E93" s="32"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6295,7 +6373,7 @@
       </c>
       <c r="B94" s="29"/>
       <c r="C94" s="30"/>
-      <c r="D94" s="33"/>
+      <c r="D94" s="29"/>
       <c r="E94" s="32"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6304,7 +6382,7 @@
       </c>
       <c r="B95" s="29"/>
       <c r="C95" s="30"/>
-      <c r="D95" s="33"/>
+      <c r="D95" s="29"/>
       <c r="E95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6313,7 +6391,7 @@
       </c>
       <c r="B96" s="29"/>
       <c r="C96" s="30"/>
-      <c r="D96" s="33"/>
+      <c r="D96" s="29"/>
       <c r="E96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6322,7 +6400,7 @@
       </c>
       <c r="B97" s="29"/>
       <c r="C97" s="30"/>
-      <c r="D97" s="33"/>
+      <c r="D97" s="29"/>
       <c r="E97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6331,7 +6409,7 @@
       </c>
       <c r="B98" s="29"/>
       <c r="C98" s="30"/>
-      <c r="D98" s="33"/>
+      <c r="D98" s="29"/>
       <c r="E98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6340,7 +6418,7 @@
       </c>
       <c r="B99" s="29"/>
       <c r="C99" s="30"/>
-      <c r="D99" s="33"/>
+      <c r="D99" s="29"/>
       <c r="E99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6349,7 +6427,7 @@
       </c>
       <c r="B100" s="29"/>
       <c r="C100" s="30"/>
-      <c r="D100" s="33"/>
+      <c r="D100" s="29"/>
       <c r="E100" s="32"/>
     </row>
   </sheetData>
@@ -6386,7 +6464,8 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10253,7 +10332,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>2</v>
@@ -10449,7 +10528,7 @@
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>

</xml_diff>